<commit_message>
feat: tema de clasificación
</commit_message>
<xml_diff>
--- a/data/02_datos_lineales_ruido.xlsx
+++ b/data/02_datos_lineales_ruido.xlsx
@@ -1,25 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documentos\modelos_ml_estudio\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3530D37-F779-4C07-B380-A89567A9AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +358,915 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75:F75"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f ca="1">A2*7+RANDBETWEEN(1,80)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f ca="1">A3*7+RANDBETWEEN(1,80)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B67" ca="1" si="0">A4*7+RANDBETWEEN(1,80)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ca="1" si="0"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ca="1" si="0"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ca="1" si="0"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ca="1" si="0"/>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ca="1" si="0"/>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="0"/>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ca="1" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ca="1" si="0"/>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" ca="1" si="0"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" ca="1" si="0"/>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ca="1" si="0"/>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ca="1" si="0"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ca="1" si="0"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ca="1" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ca="1" si="0"/>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ca="1" si="0"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ca="1" si="0"/>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ca="1" si="0"/>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ca="1" si="0"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" ca="1" si="0"/>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ca="1" si="0"/>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ca="1" si="0"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" ca="1" si="0"/>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" ca="1" si="0"/>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" ca="1" si="0"/>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" ca="1" si="0"/>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ca="1" si="0"/>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" ca="1" si="0"/>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" ca="1" si="0"/>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" ca="1" si="0"/>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" ca="1" si="0"/>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" ca="1" si="0"/>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <f t="shared" ca="1" si="0"/>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <f t="shared" ca="1" si="0"/>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <f t="shared" ca="1" si="0"/>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <f t="shared" ca="1" si="0"/>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ca="1" si="0"/>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <f t="shared" ref="B68:B100" ca="1" si="1">A68*7+RANDBETWEEN(1,80)</f>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <f t="shared" ca="1" si="1"/>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <f t="shared" ca="1" si="1"/>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <f t="shared" ca="1" si="1"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <f t="shared" ca="1" si="1"/>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <f t="shared" ca="1" si="1"/>
+        <v>566</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <f t="shared" ca="1" si="1"/>
+        <v>573</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <f t="shared" ca="1" si="1"/>
+        <v>543</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <f t="shared" ca="1" si="1"/>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <f t="shared" ca="1" si="1"/>
+        <v>574</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <f t="shared" ca="1" si="1"/>
+        <v>611</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <f t="shared" ca="1" si="1"/>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <f t="shared" ca="1" si="1"/>
+        <v>615</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <f t="shared" ca="1" si="1"/>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <f t="shared" ca="1" si="1"/>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <f t="shared" ca="1" si="1"/>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <f t="shared" ca="1" si="1"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <f t="shared" ca="1" si="1"/>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <f t="shared" ca="1" si="1"/>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <f t="shared" ca="1" si="1"/>
+        <v>674</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <f t="shared" ca="1" si="1"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <f t="shared" ca="1" si="1"/>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <f t="shared" ca="1" si="1"/>
+        <v>663</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <f t="shared" ca="1" si="1"/>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <f t="shared" ca="1" si="1"/>
+        <v>708</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <f t="shared" ca="1" si="1"/>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <f t="shared" ca="1" si="1"/>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <f t="shared" ca="1" si="1"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <f t="shared" ca="1" si="1"/>
+        <v>674</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <f t="shared" ca="1" si="1"/>
+        <v>707</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <f t="shared" ca="1" si="1"/>
+        <v>727</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <f t="shared" ca="1" si="1"/>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <f t="shared" ca="1" si="1"/>
+        <v>695</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>